<commit_message>
Update data in spreadsheet and Methodology document
Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Energy use of products.xlsx
+++ b/Energy use of products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahritchie/Desktop/data-projects/energy-use-products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E34291-5873-2340-B621-5C7A4B810033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F401EF-A143-2B4F-92DD-62FB4ACA42BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{E9F44B29-F67D-AA43-897E-E427581FB5C3}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17180" xr2:uid="{E9F44B29-F67D-AA43-897E-E427581FB5C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy" sheetId="2" r:id="rId1"/>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B239A6D3-151C-6C42-AB20-47DEE8CAFF43}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,7 +709,8 @@
     <col min="1" max="1" width="31.1640625" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1000,7 +1001,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="1">
-        <f>1/60*5</f>
+        <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E19" s="2">
@@ -1133,12 +1134,13 @@
       <c r="C28" t="s">
         <v>25</v>
       </c>
-      <c r="D28">
-        <v>0.16</v>
+      <c r="D28" s="1">
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" ref="E28" si="5">B28*D28</f>
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1195,12 +1197,13 @@
       <c r="C33" t="s">
         <v>25</v>
       </c>
-      <c r="D33">
-        <v>0.16</v>
+      <c r="D33" s="1">
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" ref="E33" si="6">B33*D33</f>
-        <v>400</v>
+        <v>416.66666666666663</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1218,12 +1221,13 @@
       <c r="C35" t="s">
         <v>25</v>
       </c>
-      <c r="D35">
-        <v>0.08</v>
-      </c>
-      <c r="E35">
-        <f>B35*D35</f>
-        <v>140</v>
+      <c r="D35" s="1">
+        <f>1/12</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" ref="E35:E45" si="7">B35*D35</f>
+        <v>145.83333333333331</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1236,12 +1240,13 @@
       <c r="C36" t="s">
         <v>25</v>
       </c>
-      <c r="D36">
-        <v>0.16</v>
-      </c>
-      <c r="E36">
-        <f>B36*D36</f>
-        <v>1520</v>
+      <c r="D36" s="1">
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="7"/>
+        <v>1583.3333333333333</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1255,12 +1260,13 @@
       <c r="C37" t="s">
         <v>25</v>
       </c>
-      <c r="D37">
-        <v>0.16</v>
+      <c r="D37" s="1">
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E37" s="2">
-        <f>B37*D37</f>
-        <v>1688.8888888888887</v>
+        <f t="shared" si="7"/>
+        <v>1759.2592592592591</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1277,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="E38">
-        <f>B38*D38</f>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
     </row>
@@ -1295,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="E39">
-        <f>B39*D39</f>
+        <f t="shared" si="7"/>
         <v>750</v>
       </c>
     </row>
@@ -1313,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="E40">
-        <f>B40*D40</f>
+        <f t="shared" si="7"/>
         <v>1500</v>
       </c>
     </row>
@@ -1331,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="E41">
-        <f>B41*D41</f>
+        <f t="shared" si="7"/>
         <v>800</v>
       </c>
     </row>
@@ -1349,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="E42">
-        <f>B42*D42</f>
+        <f t="shared" si="7"/>
         <v>2250</v>
       </c>
     </row>
@@ -1367,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="E43">
-        <f>B43*D43</f>
+        <f t="shared" si="7"/>
         <v>2700</v>
       </c>
     </row>
@@ -1385,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="E44">
-        <f>B44*D44</f>
+        <f t="shared" si="7"/>
         <v>7500</v>
       </c>
     </row>
@@ -1403,7 +1409,7 @@
         <v>1</v>
       </c>
       <c r="E45">
-        <f>B45*D45</f>
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update oven energy calculations with cycling factor and improve labels
Updated figures for Electric oven and Gas oven to account for cycling behavior (0.55 factor). Added clearer units for fixed items that show per day values. Updated methodology and change log.

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Energy use of products.xlsx
+++ b/Energy use of products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahritchie/Desktop/data-projects/energy-use-products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F401EF-A143-2B4F-92DD-62FB4ACA42BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E932A3BB-513F-B241-8586-27366F7FD331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17180" xr2:uid="{E9F44B29-F67D-AA43-897E-E427581FB5C3}"/>
+    <workbookView xWindow="21960" yWindow="2800" windowWidth="33820" windowHeight="22300" xr2:uid="{E9F44B29-F67D-AA43-897E-E427581FB5C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="77">
   <si>
     <t>Product</t>
   </si>
@@ -246,9 +246,6 @@
     <t>Gaming console (Xbox Series X)</t>
   </si>
   <si>
-    <t>Full charge</t>
-  </si>
-  <si>
     <t>Using an e-scooter</t>
   </si>
   <si>
@@ -265,6 +262,15 @@
   </si>
   <si>
     <t>Electric heat pump (3-bed house)</t>
+  </si>
+  <si>
+    <t>Vacuum cleaner (hoover)</t>
+  </si>
+  <si>
+    <t>Per day (full charge)</t>
+  </si>
+  <si>
+    <t>Per day</t>
   </si>
 </sst>
 </file>
@@ -341,6 +347,7 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
       <xxl21:absoluteUrl r:id="rId2"/>
+      <xxl21:relativeUrl r:id="rId3"/>
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Energy use of products"/>
@@ -700,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B239A6D3-151C-6C42-AB20-47DEE8CAFF43}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,7 +788,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -1022,9 +1029,9 @@
       <c r="D20">
         <v>0.5</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>1250</v>
+      <c r="E20" s="2">
+        <f>B20*D20*0.55</f>
+        <v>687.5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1040,9 +1047,9 @@
       <c r="D21">
         <v>0.5</v>
       </c>
-      <c r="E21">
-        <f t="shared" ref="E21" si="2">B21*D21</f>
-        <v>1500</v>
+      <c r="E21" s="2">
+        <f>B21*D21*0.55</f>
+        <v>825.00000000000011</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1060,7 +1067,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" ref="E22:E23" si="3">B22*D22</f>
+        <f t="shared" ref="E22:E23" si="2">B22*D22</f>
         <v>166.66666666666666</v>
       </c>
     </row>
@@ -1079,7 +1086,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>125</v>
       </c>
     </row>
@@ -1098,7 +1105,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" ref="E24" si="4">B24*D24</f>
+        <f t="shared" ref="E24" si="3">B24*D24</f>
         <v>266.66666666666663</v>
       </c>
     </row>
@@ -1106,6 +1113,9 @@
       <c r="A25" t="s">
         <v>45</v>
       </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
       <c r="E25" s="2">
         <v>275</v>
       </c>
@@ -1114,6 +1124,9 @@
       <c r="A26" t="s">
         <v>46</v>
       </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
       <c r="E26" s="2">
         <f>300*1000/365</f>
         <v>821.91780821917803</v>
@@ -1126,7 +1139,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B28">
         <v>750</v>
@@ -1139,7 +1152,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" ref="E28" si="5">B28*D28</f>
+        <f t="shared" ref="E28" si="4">B28*D28</f>
         <v>125</v>
       </c>
     </row>
@@ -1202,7 +1215,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" ref="E33" si="6">B33*D33</f>
+        <f t="shared" ref="E33" si="5">B33*D33</f>
         <v>416.66666666666663</v>
       </c>
     </row>
@@ -1226,7 +1239,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" ref="E35:E45" si="7">B35*D35</f>
+        <f t="shared" ref="E35:E45" si="6">B35*D35</f>
         <v>145.83333333333331</v>
       </c>
     </row>
@@ -1245,7 +1258,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1583.3333333333333</v>
       </c>
     </row>
@@ -1265,7 +1278,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1759.2592592592591</v>
       </c>
     </row>
@@ -1283,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="E38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
     </row>
@@ -1301,13 +1314,13 @@
         <v>1</v>
       </c>
       <c r="E39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>750</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B40">
         <v>1500</v>
@@ -1319,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="E40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1500</v>
       </c>
     </row>
@@ -1337,13 +1350,13 @@
         <v>1</v>
       </c>
       <c r="E41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>800</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B42">
         <v>2250</v>
@@ -1355,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="E42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2250</v>
       </c>
     </row>
@@ -1373,13 +1386,13 @@
         <v>1</v>
       </c>
       <c r="E43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2700</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B44">
         <v>7500</v>
@@ -1391,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="E44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>7500</v>
       </c>
     </row>
@@ -1409,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="E45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
     </row>
@@ -1431,7 +1444,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B48">
         <v>25</v>
@@ -1442,7 +1455,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B49">
         <v>150</v>
@@ -1453,7 +1466,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50">
         <v>530</v>

</xml_diff>